<commit_message>
actualizacion de extra addons
</commit_message>
<xml_diff>
--- a/extra_addons/customaddons-main/gps_bancos/reports/reporte_conciliacion.xlsx
+++ b/extra_addons/customaddons-main/gps_bancos/reports/reporte_conciliacion.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\digit\Documents\Odoo\Odoo16\extra_addons\customaddons-main\gps_bancos\reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\digit\Documents\Odoo\Odoo16\addons\customaddons-main\gps_bancos\reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A721DE2-581B-48D0-9E81-97C38A2FD172}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A71D06-E9E6-4C95-B8E7-3B057226DA53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t># LINEAS:</t>
   </si>
@@ -86,49 +86,73 @@
     <t>PÁG. : 1 DE 1</t>
   </si>
   <si>
-    <t>(=)</t>
-  </si>
-  <si>
     <t>DETALLE PARTIDAS CONCILIATORIAS</t>
   </si>
   <si>
-    <t xml:space="preserve">(-) </t>
-  </si>
-  <si>
-    <t>CHEQUES GIRADOS NO COBRADOS</t>
-  </si>
-  <si>
-    <t>N/D NO REGISTRADOS EN BANCOS</t>
-  </si>
-  <si>
-    <t>(+)</t>
-  </si>
-  <si>
-    <t>DEPÓSITOS NO EN EL BANCO</t>
-  </si>
-  <si>
-    <t>(-)</t>
-  </si>
-  <si>
-    <t>DEPÓSITOS Y  N/C NO REGIST.EN LIBROS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(+) </t>
-  </si>
-  <si>
-    <t>N/D NO REGISTRADO EN LIBROS</t>
-  </si>
-  <si>
-    <t>(+/ -)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SALDO INICIAL MESES ANTERIORES </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SALDO CONCILIACIÓN             </t>
-  </si>
-  <si>
-    <t>DIFERENCIA</t>
+    <t>MES</t>
+  </si>
+  <si>
+    <t>DIARIO</t>
+  </si>
+  <si>
+    <t># Referencia</t>
+  </si>
+  <si>
+    <t>Descr. Referencia Bancaria</t>
+  </si>
+  <si>
+    <t>MOVIMIENTOS  EN BANCOS</t>
+  </si>
+  <si>
+    <t># Cuenta:</t>
+  </si>
+  <si>
+    <t>MOVIMIENTOS POR ASIENTOS CONTABLES</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>Referencia</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Valor</t>
+  </si>
+  <si>
+    <t>Valor Con Signo</t>
+  </si>
+  <si>
+    <t>Saldo Disponible</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>Diario</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHEQUE GIRADOS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSFERENCIAS REALIZADAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">COMISIONES BANCARIAS </t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TRANSFERENCIAS RECIBIDAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DIFERENCIA </t>
   </si>
   <si>
     <t>ELABORADO POR:</t>
@@ -150,57 +174,6 @@
   </si>
   <si>
     <t>GERENTE FINANCIERO</t>
-  </si>
-  <si>
-    <t>MES</t>
-  </si>
-  <si>
-    <t>DIARIO</t>
-  </si>
-  <si>
-    <t># Referencia</t>
-  </si>
-  <si>
-    <t>Descr. Referencia Bancaria</t>
-  </si>
-  <si>
-    <t>MOVIMIENTOS  EN BANCOS</t>
-  </si>
-  <si>
-    <t># Cuenta:</t>
-  </si>
-  <si>
-    <t>MOVIMIENTOS POR ASIENTOS CONTABLES</t>
-  </si>
-  <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>Referencia</t>
-  </si>
-  <si>
-    <t>Tipo</t>
-  </si>
-  <si>
-    <t>Valor</t>
-  </si>
-  <si>
-    <t>Valor Con Signo</t>
-  </si>
-  <si>
-    <t>Saldo Disponible</t>
-  </si>
-  <si>
-    <t>Descripcion</t>
-  </si>
-  <si>
-    <t>Diario</t>
-  </si>
-  <si>
-    <t>SALDO LIBROS</t>
-  </si>
-  <si>
-    <t>SALDO SEGÚN BANCOS</t>
   </si>
 </sst>
 </file>
@@ -211,7 +184,7 @@
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="165" formatCode="_ &quot;$&quot;* #,##0.00_ ;_ &quot;$&quot;* \-#,##0.00_ ;_ &quot;$&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,25 +267,44 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
       <sz val="10"/>
       <color indexed="9"/>
       <name val="Verdana"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Verdana"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="10"/>
-      <name val="Verdana"/>
-      <charset val="134"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -534,12 +526,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -571,25 +567,24 @@
     <xf numFmtId="17" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -599,6 +594,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -608,56 +621,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="11" fillId="3" borderId="15" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -704,11 +669,39 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="165" fontId="16" fillId="3" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="3" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="3" borderId="14" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="3" borderId="15" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="3" borderId="14" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="15" fillId="3" borderId="15" xfId="6" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
+    <cellStyle name="Currency 2" xfId="4" xr:uid="{19DF103A-7045-4F32-988E-55F36F6278C6}"/>
     <cellStyle name="Millares 2" xfId="1" xr:uid="{8EE187C0-29CA-4069-8282-F57F815EC277}"/>
+    <cellStyle name="Millares 2 2" xfId="5" xr:uid="{91F047B9-4F17-44FD-A7B4-B75248F03EDF}"/>
     <cellStyle name="Moneda 2" xfId="2" xr:uid="{A202AFE0-E010-437C-9B26-072A3F65A13B}"/>
+    <cellStyle name="Moneda 2 2" xfId="6" xr:uid="{427FCF42-A552-4FD9-AC84-59C914F703FB}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="3" xr:uid="{869EB265-9715-4E2C-9D0F-DC17B133B3A5}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -725,98 +718,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>714375</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="Line 37">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF458A21-EC86-416C-AC99-F7C616EAA4E4}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeShapeType="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6635115" y="5787390"/>
-          <a:ext cx="304800" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:tailEnd type="triangle" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>695325</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="Line 38">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF681437-DE93-4269-BFD7-D7AB82C49C85}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr>
-          <a:spLocks noChangeShapeType="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6625590" y="5987415"/>
-          <a:ext cx="295275" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:round/>
-          <a:tailEnd type="triangle" w="med" len="med"/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -1179,28 +1080,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="1" customFormat="1" ht="29.55" customHeight="1">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-      <c r="K1" s="24"/>
-      <c r="L1" s="24"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
     </row>
     <row r="2" spans="1:12" ht="18">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1222,7 +1123,7 @@
     </row>
     <row r="4" spans="1:12" ht="28.8">
       <c r="A4" s="5" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>7</v>
@@ -1252,10 +1153,10 @@
         <v>6</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="L4" s="6" t="s">
-        <v>42</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1287,23 +1188,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="29.55" customHeight="1">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="24" t="s">
-        <v>43</v>
-      </c>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
     </row>
     <row r="2" spans="1:10" ht="18">
       <c r="A2" s="2" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
       <c r="E2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1328,31 +1229,31 @@
         <v>1</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>46</v>
+        <v>25</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>51</v>
+        <v>30</v>
       </c>
       <c r="I4" s="5" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>48</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1367,10 +1268,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16D6E2AB-CD9F-4E7B-A750-F6004FF7004B}">
-  <dimension ref="B1:G45"/>
+  <dimension ref="B1:G38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4"/>
@@ -1393,43 +1294,43 @@
     </row>
     <row r="2" spans="2:7" ht="16.2" customHeight="1">
       <c r="B2" s="10"/>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="45" t="s">
+      <c r="D2" s="41"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="46"/>
+      <c r="G2" s="35"/>
     </row>
     <row r="3" spans="2:7" ht="16.2" customHeight="1">
       <c r="B3" s="11"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="56"/>
-      <c r="F3" s="47" t="s">
+      <c r="C3" s="43"/>
+      <c r="D3" s="44"/>
+      <c r="E3" s="45"/>
+      <c r="F3" s="36" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="48"/>
+      <c r="G3" s="37"/>
     </row>
     <row r="4" spans="2:7" ht="16.2" customHeight="1">
       <c r="B4" s="11"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="48"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="37"/>
     </row>
     <row r="5" spans="2:7" ht="16.2" customHeight="1">
       <c r="B5" s="12"/>
-      <c r="C5" s="57"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="49" t="s">
+      <c r="C5" s="46"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="G5" s="50"/>
+      <c r="G5" s="39"/>
     </row>
     <row r="6" spans="2:7">
       <c r="B6" s="13"/>
@@ -1446,32 +1347,32 @@
       <c r="F7" s="8"/>
     </row>
     <row r="8" spans="2:7">
-      <c r="B8" s="40" t="s">
-        <v>40</v>
-      </c>
-      <c r="C8" s="40"/>
-      <c r="D8" s="40"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="40"/>
+      <c r="B8" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
     </row>
     <row r="9" spans="2:7">
-      <c r="B9" s="40"/>
-      <c r="C9" s="40"/>
-      <c r="D9" s="40"/>
-      <c r="E9" s="40"/>
-      <c r="F9" s="40"/>
-      <c r="G9" s="40"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
     </row>
     <row r="10" spans="2:7">
-      <c r="B10" s="40" t="s">
-        <v>39</v>
-      </c>
-      <c r="C10" s="40"/>
-      <c r="D10" s="40"/>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
+      <c r="B10" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="14"/>
@@ -1487,299 +1388,197 @@
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
     </row>
-    <row r="13" spans="2:7">
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+    <row r="13" spans="2:7" ht="21" customHeight="1">
+      <c r="C13" s="15"/>
+      <c r="D13" s="16"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="50"/>
     </row>
     <row r="14" spans="2:7">
-      <c r="B14" s="15" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="17"/>
+    </row>
+    <row r="15" spans="2:7" ht="26.4">
+      <c r="C15" s="15"/>
+      <c r="D15" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="41" t="s">
-        <v>55</v>
-      </c>
-      <c r="D14" s="42"/>
-      <c r="F14" s="32"/>
-      <c r="G14" s="33"/>
-    </row>
-    <row r="15" spans="2:7">
-      <c r="B15" s="16"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="18"/>
     </row>
     <row r="16" spans="2:7">
-      <c r="B16" s="16"/>
-      <c r="C16" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="D16" s="44"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="18"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="17"/>
     </row>
     <row r="17" spans="2:7">
-      <c r="B17" s="16"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="18"/>
+      <c r="C17" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="51"/>
+      <c r="G17" s="52"/>
     </row>
     <row r="18" spans="2:7">
-      <c r="B18" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>20</v>
-      </c>
-      <c r="D18" s="38"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="33"/>
+      <c r="C18" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="51"/>
+      <c r="G18" s="52"/>
     </row>
     <row r="19" spans="2:7">
-      <c r="B19" s="19"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="18"/>
+      <c r="C19" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="51"/>
+      <c r="G19" s="52"/>
     </row>
     <row r="20" spans="2:7">
-      <c r="B20" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="38" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="38"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="17"/>
     </row>
     <row r="21" spans="2:7">
-      <c r="B21" s="19"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="20"/>
+      <c r="C21" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" s="51"/>
+      <c r="G21" s="52"/>
     </row>
     <row r="22" spans="2:7">
-      <c r="B22" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="C22" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" s="38"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="17"/>
     </row>
     <row r="23" spans="2:7">
-      <c r="B23" s="19"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="20"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="19"/>
+      <c r="F23" s="51">
+        <f>+F13+F21-F17-F18-F19</f>
+        <v>0</v>
+      </c>
+      <c r="G23" s="52"/>
     </row>
     <row r="24" spans="2:7">
-      <c r="B24" s="15" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="38" t="s">
-        <v>25</v>
-      </c>
-      <c r="D24" s="38"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="33"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="19"/>
+      <c r="F24" s="54"/>
+      <c r="G24" s="55"/>
     </row>
     <row r="25" spans="2:7">
-      <c r="B25" s="19"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="20"/>
-    </row>
-    <row r="26" spans="2:7">
-      <c r="B26" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="38"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33"/>
-    </row>
-    <row r="27" spans="2:7">
-      <c r="B27" s="16"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="20"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F25" s="53">
+        <f>+F23-F24</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="53"/>
     </row>
     <row r="28" spans="2:7">
-      <c r="B28" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="C28" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="D28" s="38"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="32"/>
-      <c r="G28" s="33"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="56"/>
+      <c r="G28" s="56"/>
     </row>
     <row r="29" spans="2:7">
-      <c r="B29" s="16"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="20"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="56"/>
     </row>
     <row r="30" spans="2:7">
-      <c r="B30" s="16"/>
-      <c r="C30" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="D30" s="39"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="32"/>
-      <c r="G30" s="33"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
     </row>
     <row r="31" spans="2:7">
-      <c r="B31" s="16"/>
-      <c r="C31" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="D31" s="31"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="32"/>
-      <c r="G31" s="33"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
     </row>
     <row r="32" spans="2:7">
-      <c r="B32" s="8"/>
-      <c r="C32" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="34"/>
+      <c r="B32" s="56"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="G32" s="56"/>
     </row>
     <row r="33" spans="2:7">
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-    </row>
-    <row r="34" spans="2:7">
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-      <c r="F34" s="8"/>
-    </row>
-    <row r="35" spans="2:7">
-      <c r="B35" s="8"/>
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="G33" s="56"/>
     </row>
     <row r="36" spans="2:7">
-      <c r="B36" s="8"/>
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-      <c r="F36" s="8"/>
+      <c r="B36" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="28"/>
+      <c r="D36" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" s="29"/>
+      <c r="F36" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="G36" s="29"/>
     </row>
     <row r="37" spans="2:7">
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-      <c r="F37" s="8"/>
+      <c r="B37" s="30"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="30"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="30" t="s">
+        <v>43</v>
+      </c>
+      <c r="G37" s="32"/>
     </row>
     <row r="38" spans="2:7">
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-      <c r="F38" s="8"/>
-    </row>
-    <row r="39" spans="2:7">
-      <c r="B39" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="C39" s="36"/>
-      <c r="D39" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="E39" s="37"/>
-      <c r="F39" s="35" t="s">
-        <v>34</v>
-      </c>
-      <c r="G39" s="37"/>
-    </row>
-    <row r="40" spans="2:7">
-      <c r="B40" s="25"/>
-      <c r="C40" s="26"/>
-      <c r="D40" s="25"/>
-      <c r="E40" s="27"/>
-      <c r="F40" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="G40" s="27"/>
-    </row>
-    <row r="41" spans="2:7">
-      <c r="B41" s="28" t="s">
-        <v>36</v>
-      </c>
-      <c r="C41" s="29"/>
-      <c r="D41" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="E41" s="30"/>
-      <c r="F41" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="G41" s="30"/>
-    </row>
-    <row r="42" spans="2:7">
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="8"/>
-    </row>
-    <row r="43" spans="2:7">
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-    </row>
-    <row r="44" spans="2:7">
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-      <c r="F44" s="8"/>
-    </row>
-    <row r="45" spans="2:7">
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="F45" s="8"/>
+      <c r="B38" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="25"/>
+      <c r="D38" s="24" t="s">
+        <v>45</v>
+      </c>
+      <c r="E38" s="26"/>
+      <c r="F38" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G38" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="37">
+  <mergeCells count="26">
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F17:G17"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="F23:G23"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="B10:G10"/>
     <mergeCell ref="B8:G9"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F3:G3"/>
@@ -1787,36 +1586,16 @@
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="C2:E3"/>
     <mergeCell ref="C4:E5"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C18:D18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="C22:D22"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="C24:D24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="F26:G26"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="F28:G28"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="F30:G30"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="F31:G31"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="F41:G41"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="B28:G33"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="F37:G37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>